<commit_message>
hand optimize ANN XOR ready
</commit_message>
<xml_diff>
--- a/AI/annxor.xlsx
+++ b/AI/annxor.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="work" sheetId="1" r:id="rId1"/>
+    <sheet name="answer" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>x1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,6 +111,26 @@
   </si>
   <si>
     <t>TS4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2w1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2W2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2W3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L2W4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>output</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -171,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -397,19 +418,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -466,6 +474,98 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -476,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -508,21 +608,33 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -803,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:AB11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="W11" sqref="W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -825,18 +937,644 @@
     <col min="12" max="12" width="4.75" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
     <col min="14" max="14" width="4.5" customWidth="1"/>
-    <col min="15" max="15" width="6.5" customWidth="1"/>
+    <col min="15" max="15" width="4.75" customWidth="1"/>
     <col min="16" max="16" width="3.875" customWidth="1"/>
     <col min="17" max="17" width="4.5" customWidth="1"/>
     <col min="18" max="18" width="5" customWidth="1"/>
-    <col min="19" max="19" width="4.75" customWidth="1"/>
+    <col min="19" max="19" width="3.75" customWidth="1"/>
+    <col min="20" max="20" width="4.5" customWidth="1"/>
+    <col min="21" max="21" width="4.875" customWidth="1"/>
+    <col min="22" max="22" width="5.25" customWidth="1"/>
+    <col min="23" max="23" width="4.125" customWidth="1"/>
+    <col min="24" max="24" width="4.75" customWidth="1"/>
+    <col min="25" max="26" width="5.5" customWidth="1"/>
+    <col min="27" max="27" width="5.375" customWidth="1"/>
+    <col min="28" max="28" width="6.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="T1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="54" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="48">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0</v>
+      </c>
+      <c r="F2" s="15">
+        <v>0</v>
+      </c>
+      <c r="G2" s="16">
+        <v>0</v>
+      </c>
+      <c r="H2" s="13">
+        <v>-1</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15">
+        <v>0</v>
+      </c>
+      <c r="K2" s="16">
+        <v>0</v>
+      </c>
+      <c r="L2" s="13">
+        <v>-1</v>
+      </c>
+      <c r="M2" s="14">
+        <v>0</v>
+      </c>
+      <c r="N2" s="15">
+        <v>0</v>
+      </c>
+      <c r="O2" s="45">
+        <v>0</v>
+      </c>
+      <c r="P2" s="32">
+        <f>$A2*D2+$B2*H2+$C2*L2</f>
+        <v>1</v>
+      </c>
+      <c r="Q2" s="8">
+        <f>$A2*E2+$B2*I2+$C2*M2</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="18">
+        <f>$A2*F2+$B2*J2+$C2*N2</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="30">
+        <f>$A2*G2+$B2*K2+$C2*O2</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="42">
+        <v>1</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="43">
+        <v>0</v>
+      </c>
+      <c r="X2" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="56">
+        <f>X2*T2+Y2*U2+Z2*V2+AA2*W2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="37">
+        <f>A$2</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:O5" si="0">D$2</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M3" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N3" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="32">
+        <f t="shared" ref="P3:P5" si="1">$A3*D3+$B3*H3+$C3*L3</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8">
+        <f t="shared" ref="Q3:Q5" si="2">$A3*E3+$B3*I3+$C3*M3</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="18">
+        <f t="shared" ref="R3:R5" si="3">$A3*F3+$B3*J3+$C3*N3</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="30">
+        <f t="shared" ref="S3:S5" si="4">$A3*G3+$B3*K3+$C3*O3</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="37">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="38">
+        <v>0</v>
+      </c>
+      <c r="X3" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="56">
+        <f t="shared" ref="AB3:AB5" si="5">X3*T3+Y3*U3+Z3*V3+AA3*W3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="37">
+        <f>A$2</f>
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M4" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="37">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="38">
+        <v>0</v>
+      </c>
+      <c r="X4" s="50">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="56">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37">
+        <f>A$2</f>
+        <v>1</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1</v>
+      </c>
+      <c r="C5" s="40">
+        <v>1</v>
+      </c>
+      <c r="D5" s="46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H5" s="46">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L5" s="46">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="M5" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N5" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="33">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="Q5" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="35">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="39">
+        <v>0</v>
+      </c>
+      <c r="U5" s="40">
+        <v>0</v>
+      </c>
+      <c r="V5" s="40">
+        <v>0</v>
+      </c>
+      <c r="W5" s="41">
+        <v>1</v>
+      </c>
+      <c r="X5" s="51">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="52">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="52">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="52">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="21">
+        <f>D2</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="19">
+        <f>E2</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="27">
+        <f>F2</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="22">
+        <f>G2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" s="23">
+        <f>H2</f>
+        <v>-1</v>
+      </c>
+      <c r="G9" s="3">
+        <f>I2</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="4">
+        <f>J2</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="24">
+        <f>K2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="25">
+        <f>L2</f>
+        <v>-1</v>
+      </c>
+      <c r="G10" s="20">
+        <f>M2</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="28">
+        <f>N2</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="26">
+        <f>O2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B0E69D4-4E78-4AA5-854F-C181FE5D72BA}">
+  <dimension ref="A1:AB11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AB5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="4.5" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="4.25" customWidth="1"/>
+    <col min="5" max="5" width="5.25" customWidth="1"/>
+    <col min="6" max="6" width="4.125" customWidth="1"/>
+    <col min="7" max="7" width="4.5" customWidth="1"/>
+    <col min="8" max="8" width="4.375" customWidth="1"/>
+    <col min="9" max="9" width="4.875" customWidth="1"/>
+    <col min="10" max="10" width="4.75" customWidth="1"/>
+    <col min="11" max="11" width="5.125" customWidth="1"/>
+    <col min="12" max="12" width="4.75" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="4.5" customWidth="1"/>
+    <col min="15" max="15" width="4.75" customWidth="1"/>
+    <col min="16" max="16" width="3.875" customWidth="1"/>
+    <col min="17" max="17" width="4.5" customWidth="1"/>
+    <col min="18" max="18" width="5" customWidth="1"/>
+    <col min="19" max="19" width="3.75" customWidth="1"/>
     <col min="20" max="20" width="4.5" customWidth="1"/>
     <col min="21" max="21" width="4.875" customWidth="1"/>
     <col min="22" max="22" width="5.25" customWidth="1"/>
     <col min="23" max="23" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -879,10 +1617,10 @@
       <c r="N1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="31" t="s">
         <v>10</v>
       </c>
       <c r="Q1" s="14" t="s">
@@ -903,61 +1641,74 @@
       <c r="V1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="W1" s="44" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="49" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="49" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+    <row r="2" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="42">
         <v>1</v>
       </c>
       <c r="B2" s="6">
         <v>0</v>
       </c>
-      <c r="C2" s="6">
-        <v>0</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8">
+      <c r="C2" s="48">
+        <v>0</v>
+      </c>
+      <c r="D2" s="31">
+        <v>10</v>
+      </c>
+      <c r="E2" s="14">
         <v>0.2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="15">
         <v>-1</v>
       </c>
-      <c r="G2" s="10">
-        <v>-2</v>
-      </c>
-      <c r="H2" s="7">
-        <f>F9</f>
-        <v>-1</v>
-      </c>
-      <c r="I2" s="8">
-        <v>-1</v>
-      </c>
-      <c r="J2" s="9">
-        <v>2</v>
-      </c>
-      <c r="K2" s="10">
-        <v>2</v>
-      </c>
-      <c r="L2" s="7">
-        <f>F10</f>
-        <v>-1</v>
-      </c>
-      <c r="M2" s="8">
-        <v>2</v>
-      </c>
-      <c r="N2" s="9">
-        <v>-1</v>
-      </c>
-      <c r="O2" s="30">
-        <v>2</v>
-      </c>
-      <c r="P2" s="33">
+      <c r="G2" s="16">
+        <v>-20</v>
+      </c>
+      <c r="H2" s="13">
+        <v>-10</v>
+      </c>
+      <c r="I2" s="14">
+        <v>-20</v>
+      </c>
+      <c r="J2" s="15">
+        <v>20</v>
+      </c>
+      <c r="K2" s="16">
+        <v>20</v>
+      </c>
+      <c r="L2" s="13">
+        <v>-10</v>
+      </c>
+      <c r="M2" s="14">
+        <v>20</v>
+      </c>
+      <c r="N2" s="15">
+        <v>-20</v>
+      </c>
+      <c r="O2" s="45">
+        <v>20</v>
+      </c>
+      <c r="P2" s="32">
         <f>$A2*D2+$B2*H2+$C2*L2</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q2" s="8">
         <f>$A2*E2+$B2*I2+$C2*M2</f>
@@ -969,9 +1720,9 @@
       </c>
       <c r="S2" s="30">
         <f>$A2*G2+$B2*K2+$C2*O2</f>
-        <v>-2</v>
-      </c>
-      <c r="T2" s="43">
+        <v>-20</v>
+      </c>
+      <c r="T2" s="42">
         <v>1</v>
       </c>
       <c r="U2" s="6">
@@ -980,12 +1731,28 @@
       <c r="V2" s="6">
         <v>0</v>
       </c>
-      <c r="W2" s="44">
+      <c r="W2" s="43">
+        <v>0</v>
+      </c>
+      <c r="X2" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="49">
+        <f>X2*T2+Y2*U2+Z2*V2+AA2*W2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A3" s="37">
         <v>1</v>
       </c>
       <c r="B3" s="1">
@@ -994,225 +1761,305 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
-        <f>D$2</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="7">
+        <f t="shared" ref="D3:O5" si="0">D$2</f>
+        <v>10</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G3" s="5">
-        <v>-2</v>
-      </c>
-      <c r="H3" s="2">
+      <c r="G3" s="10">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="H3" s="7">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="I3" s="8">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="J3" s="9">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K3" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="M3" s="8">
+        <v>20</v>
+      </c>
+      <c r="N3" s="9">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P3" s="32">
+        <f t="shared" ref="P3:S5" si="1">$A3*D3+$B3*H3+$C3*L3</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8">
+        <f t="shared" si="1"/>
+        <v>20.2</v>
+      </c>
+      <c r="R3" s="18">
+        <f t="shared" si="1"/>
+        <v>-21</v>
+      </c>
+      <c r="S3" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T3" s="37">
+        <v>0</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>0</v>
+      </c>
+      <c r="W3" s="38">
+        <v>0</v>
+      </c>
+      <c r="X3" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="49">
+        <f t="shared" ref="AB3:AB5" si="2">X3*T3+Y3*U3+Z3*V3+AA3*W3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A4" s="37">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="I3" s="3">
-        <v>-1</v>
-      </c>
-      <c r="J3" s="4">
-        <v>2</v>
-      </c>
-      <c r="K3" s="5">
-        <v>2</v>
-      </c>
-      <c r="L3" s="2">
-        <v>-1</v>
-      </c>
-      <c r="M3" s="3">
-        <v>2</v>
-      </c>
-      <c r="N3" s="4">
-        <v>-1</v>
-      </c>
-      <c r="O3" s="31">
-        <v>2</v>
-      </c>
-      <c r="P3" s="33">
-        <f t="shared" ref="P3:P5" si="0">$A3*D3+$B3*H3+$C3*L3</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="8">
-        <f t="shared" ref="Q3:Q5" si="1">$A3*E3+$B3*I3+$C3*M3</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="R3" s="18">
-        <f t="shared" ref="R3:R5" si="2">$A3*F3+$B3*J3+$C3*N3</f>
-        <v>-2</v>
-      </c>
-      <c r="S3" s="30">
-        <f t="shared" ref="S3:S5" si="3">$A3*G3+$B3*K3+$C3*O3</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="38">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>1</v>
-      </c>
-      <c r="V3" s="1">
-        <v>0</v>
-      </c>
-      <c r="W3" s="39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <f>D$2</f>
-        <v>1</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F4" s="4">
-        <v>-1</v>
-      </c>
       <c r="G4" s="5">
-        <v>-2</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="H4" s="2">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>-10</v>
       </c>
       <c r="I4" s="3">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="J4" s="4">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="K4" s="5">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="L4" s="2">
-        <v>-1</v>
+        <f t="shared" si="0"/>
+        <v>-10</v>
       </c>
       <c r="M4" s="3">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="N4" s="4">
-        <v>-1</v>
-      </c>
-      <c r="O4" s="31">
-        <v>2</v>
-      </c>
-      <c r="P4" s="33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="O4" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P4" s="32">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q4" s="8">
         <f t="shared" si="1"/>
-        <v>-0.8</v>
+        <v>-19.8</v>
       </c>
       <c r="R4" s="18">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="S4" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="37">
+        <v>0</v>
+      </c>
+      <c r="U4" s="1">
+        <v>0</v>
+      </c>
+      <c r="V4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="38">
+        <v>0</v>
+      </c>
+      <c r="X4" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="49">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="S4" s="30">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T4" s="38">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-      <c r="V4" s="1">
-        <v>1</v>
-      </c>
-      <c r="W4" s="39">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <f>D$2</f>
-        <v>1</v>
-      </c>
-      <c r="E5" s="3">
+    <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39">
+        <v>1</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1</v>
+      </c>
+      <c r="C5" s="40">
+        <v>1</v>
+      </c>
+      <c r="D5" s="46">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E5" s="20">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="28">
+        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
-      <c r="G5" s="5">
-        <v>-2</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" s="47">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="H5" s="46">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="I5" s="20">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="J5" s="28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K5" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="L5" s="46">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="M5" s="20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="N5" s="28">
+        <f t="shared" si="0"/>
+        <v>-20</v>
+      </c>
+      <c r="O5" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="P5" s="33">
+        <f t="shared" si="1"/>
+        <v>-10</v>
+      </c>
+      <c r="Q5" s="34">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="R5" s="35">
+        <f t="shared" si="1"/>
         <v>-1</v>
       </c>
-      <c r="I5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="J5" s="4">
-        <v>2</v>
-      </c>
-      <c r="K5" s="5">
-        <v>2</v>
-      </c>
-      <c r="L5" s="2">
-        <v>-1</v>
-      </c>
-      <c r="M5" s="3">
-        <v>2</v>
-      </c>
-      <c r="N5" s="4">
-        <v>-1</v>
-      </c>
-      <c r="O5" s="31">
-        <v>2</v>
-      </c>
-      <c r="P5" s="34">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="Q5" s="35">
+      <c r="S5" s="36">
         <f t="shared" si="1"/>
-        <v>1.2</v>
-      </c>
-      <c r="R5" s="36">
+        <v>20</v>
+      </c>
+      <c r="T5" s="39">
+        <v>0</v>
+      </c>
+      <c r="U5" s="40">
+        <v>0</v>
+      </c>
+      <c r="V5" s="40">
+        <v>0</v>
+      </c>
+      <c r="W5" s="41">
+        <v>1</v>
+      </c>
+      <c r="X5" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="49">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="49">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="49">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="49">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S5" s="37">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="T5" s="40">
-        <v>0</v>
-      </c>
-      <c r="U5" s="41">
-        <v>0</v>
-      </c>
-      <c r="V5" s="41">
-        <v>0</v>
-      </c>
-      <c r="W5" s="42">
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>15</v>
       </c>
@@ -1226,58 +2073,70 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="21">
-        <v>1</v>
+        <f>D2</f>
+        <v>10</v>
       </c>
       <c r="G8" s="19">
+        <f>E2</f>
         <v>0.2</v>
       </c>
       <c r="H8" s="27">
+        <f>F2</f>
         <v>-1</v>
       </c>
       <c r="I8" s="22">
-        <v>-2</v>
+        <f>G2</f>
+        <v>-20</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>2</v>
       </c>
       <c r="F9" s="23">
-        <v>-1</v>
+        <f>H2</f>
+        <v>-10</v>
       </c>
       <c r="G9" s="3">
-        <v>-1</v>
+        <f>I2</f>
+        <v>-20</v>
       </c>
       <c r="H9" s="4">
-        <v>2</v>
+        <f>J2</f>
+        <v>20</v>
       </c>
       <c r="I9" s="24">
-        <v>2</v>
+        <f>K2</f>
+        <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="25">
-        <v>-1</v>
+        <f>L2</f>
+        <v>-10</v>
       </c>
       <c r="G10" s="20">
-        <v>2</v>
+        <f>M2</f>
+        <v>20</v>
       </c>
       <c r="H10" s="28">
-        <v>-1</v>
+        <f>N2</f>
+        <v>-20</v>
       </c>
       <c r="I10" s="26">
-        <v>2</v>
+        <f>O2</f>
+        <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
         <v>6</v>
       </c>

</xml_diff>